<commit_message>
mainly dimple level 1, 2
</commit_message>
<xml_diff>
--- a/Mould_Database/Mould_DB.xlsx
+++ b/Mould_Database/Mould_DB.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user01\Documents\kurahashi nobuaki\LaTeX\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6EA6551-F26E-4D02-8D2B-E42900B35F2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{690E1EB1-ED7C-4174-9C86-0D5AA57F2164}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19020" windowHeight="15600" tabRatio="638" firstSheet="13" activeTab="15" xr2:uid="{331D296A-DE97-4357-9338-22F5C8F49D08}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20085" windowHeight="15600" tabRatio="638" firstSheet="13" activeTab="15" xr2:uid="{331D296A-DE97-4357-9338-22F5C8F49D08}"/>
   </bookViews>
   <sheets>
     <sheet name="master" sheetId="2" r:id="rId1"/>
@@ -15894,9 +15894,7 @@
   <sheetPr codeName="Sheet16"/>
   <dimension ref="A1:R170"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.4"/>
   <cols>
@@ -19166,7 +19164,7 @@
     </row>
     <row r="96" spans="6:14" x14ac:dyDescent="0.4">
       <c r="K96" s="55">
-        <f>ROW(K96)</f>
+        <f t="shared" ref="K96:K103" si="3">ROW(K96)</f>
         <v>96</v>
       </c>
       <c r="L96" s="97" t="s">
@@ -19182,7 +19180,7 @@
     </row>
     <row r="97" spans="11:14" x14ac:dyDescent="0.4">
       <c r="K97" s="55">
-        <f>ROW(K97)</f>
+        <f t="shared" si="3"/>
         <v>97</v>
       </c>
       <c r="L97" s="97" t="s">
@@ -19198,7 +19196,7 @@
     </row>
     <row r="98" spans="11:14" x14ac:dyDescent="0.4">
       <c r="K98" s="55">
-        <f>ROW(K98)</f>
+        <f t="shared" si="3"/>
         <v>98</v>
       </c>
       <c r="L98" s="97" t="s">
@@ -19214,7 +19212,7 @@
     </row>
     <row r="99" spans="11:14" x14ac:dyDescent="0.4">
       <c r="K99" s="55">
-        <f>ROW(K99)</f>
+        <f t="shared" si="3"/>
         <v>99</v>
       </c>
       <c r="L99" s="97" t="s">
@@ -19230,7 +19228,7 @@
     </row>
     <row r="100" spans="11:14" x14ac:dyDescent="0.4">
       <c r="K100" s="55">
-        <f>ROW(K100)</f>
+        <f t="shared" si="3"/>
         <v>100</v>
       </c>
       <c r="L100" s="97" t="s">
@@ -19246,7 +19244,7 @@
     </row>
     <row r="101" spans="11:14" x14ac:dyDescent="0.4">
       <c r="K101" s="55">
-        <f>ROW(K101)</f>
+        <f t="shared" si="3"/>
         <v>101</v>
       </c>
       <c r="L101" s="97" t="s">
@@ -19262,7 +19260,7 @@
     </row>
     <row r="102" spans="11:14" x14ac:dyDescent="0.4">
       <c r="K102" s="55">
-        <f>ROW(K102)</f>
+        <f t="shared" si="3"/>
         <v>102</v>
       </c>
       <c r="L102" s="97" t="s">
@@ -19278,7 +19276,7 @@
     </row>
     <row r="103" spans="11:14" x14ac:dyDescent="0.4">
       <c r="K103" s="55">
-        <f>ROW(K103)</f>
+        <f t="shared" si="3"/>
         <v>103</v>
       </c>
       <c r="L103" s="97" t="s">
@@ -20082,7 +20080,7 @@
     </row>
     <row r="155" spans="11:14" x14ac:dyDescent="0.4">
       <c r="K155" s="55">
-        <f t="shared" ref="K155" si="3">ROW(K155)</f>
+        <f t="shared" ref="K155" si="4">ROW(K155)</f>
         <v>155</v>
       </c>
       <c r="L155" s="97" t="s">
@@ -20283,7 +20281,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation imeMode="disabled" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C57:C66 H78 N128:N141 C3:C31 C46:C49 C52:C55 H54:H72 G1:G1048576 H80:H95" xr:uid="{5A8FA8E9-E7FC-48D2-B40E-E90D3C7D1F03}"/>
+    <dataValidation imeMode="disabled" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C57:C66 H78 N128:N141 C3:C31 C46:C49 C52:C55 H54:H72 H80:H95 G1:G1048576" xr:uid="{5A8FA8E9-E7FC-48D2-B40E-E90D3C7D1F03}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -20295,7 +20293,9 @@
   <sheetPr codeName="Sheet17"/>
   <dimension ref="A1:O42"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.4"/>
   <cols>

</xml_diff>

<commit_message>
fix prgs for dimple positions
</commit_message>
<xml_diff>
--- a/Mould_Database/Mould_DB.xlsx
+++ b/Mould_Database/Mould_DB.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gm001\Documents\GitHub\mould_moji\Mould_Database\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user01\Documents\GitHub\mould\Mould_Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E96A9A0-C4FE-4E88-A070-439A14547280}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CE051F0-33B1-4F57-9D32-5F57842F6583}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-37470" yWindow="-2700" windowWidth="19770" windowHeight="21600" tabRatio="638" firstSheet="13" activeTab="15" xr2:uid="{331D296A-DE97-4357-9338-22F5C8F49D08}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19305" windowHeight="15600" tabRatio="638" firstSheet="13" activeTab="15" xr2:uid="{331D296A-DE97-4357-9338-22F5C8F49D08}"/>
   </bookViews>
   <sheets>
     <sheet name="master" sheetId="2" r:id="rId1"/>
@@ -36,19 +36,28 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
   <futureMetadata name="XLDAPR" count="1">
     <bk>
       <extLst>
-        <ext xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray" uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
           <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
         </ext>
       </extLst>
@@ -13023,6 +13032,118 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
@@ -13237,118 +13358,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
         </patternFill>
       </fill>
     </dxf>
@@ -15825,71 +15834,71 @@
   </sheetData>
   <phoneticPr fontId="1"/>
   <conditionalFormatting sqref="C3">
-    <cfRule type="expression" dxfId="54" priority="6">
+    <cfRule type="expression" dxfId="16" priority="6">
       <formula>G9^2&lt;4*G10^2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4">
-    <cfRule type="expression" dxfId="53" priority="5">
+    <cfRule type="expression" dxfId="15" priority="5">
       <formula>$C$4&lt;=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C5">
-    <cfRule type="expression" dxfId="52" priority="1">
+    <cfRule type="expression" dxfId="14" priority="1">
       <formula>C5&lt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6">
-    <cfRule type="expression" dxfId="51" priority="10">
+    <cfRule type="expression" dxfId="13" priority="10">
       <formula>OR(C5&gt;C6, C6&lt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7">
-    <cfRule type="expression" dxfId="50" priority="9">
+    <cfRule type="expression" dxfId="12" priority="9">
       <formula>AND(C7&lt;&gt;330, C7&lt;&gt;270, C7&lt;&gt;250)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="expression" dxfId="49" priority="8">
+    <cfRule type="expression" dxfId="11" priority="8">
       <formula>C8&lt;&gt;40</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9">
-    <cfRule type="expression" dxfId="48" priority="7">
+    <cfRule type="expression" dxfId="10" priority="7">
       <formula>C9&lt;&gt;100</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K3:K4">
-    <cfRule type="expression" dxfId="47" priority="15">
+    <cfRule type="expression" dxfId="9" priority="15">
       <formula>OR(($K$8&gt;($C$5+$C$6-2*$C$7)),$K$3&lt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M3:M32">
-    <cfRule type="expression" dxfId="46" priority="2">
+    <cfRule type="expression" dxfId="8" priority="2">
       <formula>Q3&gt;=1000000</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="45" priority="13">
+    <cfRule type="expression" dxfId="7" priority="13">
       <formula>Q3=MIN($Q$3:$Q32)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O3:O32">
-    <cfRule type="expression" dxfId="44" priority="3">
+    <cfRule type="expression" dxfId="6" priority="3">
       <formula>Q3&gt;=1000000</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="43" priority="12">
+    <cfRule type="expression" dxfId="5" priority="12">
       <formula>Q3=MIN($Q$3:$Q32)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P3:P32">
-    <cfRule type="expression" dxfId="42" priority="4">
+    <cfRule type="expression" dxfId="4" priority="4">
       <formula>Q3&gt;=1000000</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="41" priority="11">
+    <cfRule type="expression" dxfId="3" priority="11">
       <formula>Q3=MIN($Q$3:$Q32)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R3:R32">
-    <cfRule type="expression" dxfId="40" priority="14">
+    <cfRule type="expression" dxfId="2" priority="14">
       <formula>Q3=MIN($Q$3:$Q32)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -15905,7 +15914,9 @@
   <sheetPr codeName="Sheet16"/>
   <dimension ref="A1:R170"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="I76" sqref="I76"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.4"/>
   <cols>
@@ -16181,8 +16192,8 @@
         <v>0.64200000000000002</v>
       </c>
       <c r="I7" s="82">
-        <f>$C$66+$H$7</f>
-        <v>0.71499999999999997</v>
+        <f>-$C$66+$H$7</f>
+        <v>0.56900000000000006</v>
       </c>
       <c r="K7" s="55">
         <f t="shared" si="0"/>
@@ -16222,8 +16233,8 @@
         <v>1</v>
       </c>
       <c r="I8" s="108">
-        <f>$C$66+$H$8</f>
-        <v>1.073</v>
+        <f>-$C$66+$H$8</f>
+        <v>0.92700000000000005</v>
       </c>
       <c r="K8" s="55">
         <f t="shared" si="0"/>
@@ -18586,8 +18597,8 @@
         <v>2.7719999999999998</v>
       </c>
       <c r="I74" s="82">
-        <f ca="1">$C$66+$H$74</f>
-        <v>2.8449999999999998</v>
+        <f ca="1">-$C$66+$H$74</f>
+        <v>2.6989999999999998</v>
       </c>
       <c r="K74" s="55">
         <f t="shared" si="2"/>
@@ -18650,8 +18661,8 @@
         <v>2.4501075579837424</v>
       </c>
       <c r="I76" s="108">
-        <f ca="1">$C$66+$H$76</f>
-        <v>2.5231075579837423</v>
+        <f ca="1">-$C$66+$H$76</f>
+        <v>2.3771075579837424</v>
       </c>
       <c r="K76" s="55">
         <f t="shared" si="2"/>
@@ -20119,186 +20130,186 @@
   </sheetData>
   <phoneticPr fontId="1"/>
   <conditionalFormatting sqref="C3">
-    <cfRule type="expression" dxfId="0" priority="123">
+    <cfRule type="expression" dxfId="54" priority="123">
       <formula>$C$3&gt;2*N151</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4">
-    <cfRule type="expression" dxfId="37" priority="43">
+    <cfRule type="expression" dxfId="53" priority="43">
       <formula>C4&lt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6">
-    <cfRule type="expression" dxfId="36" priority="19">
+    <cfRule type="expression" dxfId="52" priority="19">
       <formula>$C$6&lt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9">
-    <cfRule type="expression" dxfId="35" priority="47">
+    <cfRule type="expression" dxfId="51" priority="47">
       <formula>$C$9&lt;=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10:C11">
-    <cfRule type="expression" dxfId="34" priority="20">
+    <cfRule type="expression" dxfId="50" priority="20">
       <formula>$C$10&lt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15">
-    <cfRule type="expression" dxfId="33" priority="98">
+    <cfRule type="expression" dxfId="49" priority="98">
       <formula>OR(C15&lt;=0, C15&gt;Q2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="expression" dxfId="32" priority="42">
+    <cfRule type="expression" dxfId="48" priority="42">
       <formula>C35&lt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="expression" dxfId="31" priority="57">
+    <cfRule type="expression" dxfId="47" priority="57">
       <formula>OR($C$36&lt;0, $C$36&gt;=$C$9)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="expression" dxfId="30" priority="16">
+    <cfRule type="expression" dxfId="46" priority="16">
       <formula>OR($C$37&lt;0, $C$37&gt;=$C$10)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38">
-    <cfRule type="expression" dxfId="29" priority="120">
+    <cfRule type="expression" dxfId="45" priority="120">
       <formula>OR(C38&lt;0, C38&gt;=C9)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C39">
-    <cfRule type="expression" dxfId="28" priority="127">
+    <cfRule type="expression" dxfId="44" priority="127">
       <formula>OR(C39&lt;0, C39&gt;=C4)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C42">
-    <cfRule type="expression" dxfId="27" priority="128">
+    <cfRule type="expression" dxfId="43" priority="128">
       <formula>OR(C42&lt;0, C42&gt;=C4)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C59">
-    <cfRule type="expression" dxfId="26" priority="51">
+    <cfRule type="expression" dxfId="42" priority="51">
       <formula>AND(C59&lt;&gt;330, C59&lt;&gt;270, C59&lt;&gt;250)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C60">
-    <cfRule type="expression" dxfId="25" priority="50">
+    <cfRule type="expression" dxfId="41" priority="50">
       <formula>C60&lt;&gt;40</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C63">
-    <cfRule type="expression" dxfId="24" priority="27">
+    <cfRule type="expression" dxfId="40" priority="27">
       <formula>OR(C63&gt;0, ABS(ABS(C63)-740)&gt;=1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C64">
-    <cfRule type="expression" dxfId="23" priority="40">
+    <cfRule type="expression" dxfId="39" priority="40">
       <formula>OR(C64&gt;0, ABS(ABS(C64)-550)&gt;=1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C65">
-    <cfRule type="expression" dxfId="22" priority="33">
+    <cfRule type="expression" dxfId="38" priority="33">
       <formula>OR(C65&gt;0, ABS(ABS(C65)-1150)&gt;=1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C66">
-    <cfRule type="expression" dxfId="21" priority="39">
+    <cfRule type="expression" dxfId="37" priority="39">
       <formula>OR(ABS(C66)&gt;=0.2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H48">
-    <cfRule type="expression" dxfId="20" priority="23">
+    <cfRule type="expression" dxfId="36" priority="23">
       <formula>OR($H$48&lt;=1, INT($H$48)&lt;&gt;$H$48)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H52">
-    <cfRule type="expression" dxfId="19" priority="15">
+    <cfRule type="expression" dxfId="35" priority="15">
       <formula>ISERROR(INDIRECT($H$52&amp;"!$G$45"))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C25">
-    <cfRule type="expression" dxfId="18" priority="236">
+    <cfRule type="expression" dxfId="34" priority="236">
       <formula>OR(C25-QUOTIENT(C25,1)&lt;&gt;0, C25&lt;0, C25&gt;$C$67)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H50">
-    <cfRule type="expression" dxfId="17" priority="11">
+    <cfRule type="expression" dxfId="33" priority="11">
       <formula>$H$50&lt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H78 H51:H52 H54:H72">
-    <cfRule type="expression" dxfId="16" priority="10">
+    <cfRule type="expression" dxfId="32" priority="10">
       <formula>$H$51&lt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C23">
-    <cfRule type="expression" dxfId="15" priority="254">
+    <cfRule type="expression" dxfId="31" priority="254">
       <formula>OR($C$23&lt;=0, MOD($C$23,$C$22)&lt;&gt;0, $C$23&gt;=#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C26">
-    <cfRule type="expression" dxfId="14" priority="262">
+    <cfRule type="expression" dxfId="30" priority="262">
       <formula>OR($C$26&lt;=0, $C$26&gt;=MIN($C$23, $C$24))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N128:N133">
-    <cfRule type="expression" dxfId="13" priority="9">
+    <cfRule type="expression" dxfId="29" priority="9">
       <formula>$H$51&lt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N134:N141">
-    <cfRule type="expression" dxfId="12" priority="8">
+    <cfRule type="expression" dxfId="28" priority="8">
       <formula>$H$51&lt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C16">
-    <cfRule type="expression" dxfId="11" priority="274">
+    <cfRule type="expression" dxfId="27" priority="274">
       <formula>OR(C16&lt;=0, C16+C15&gt;Q2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G1048576">
-    <cfRule type="expression" dxfId="10" priority="3">
+    <cfRule type="expression" dxfId="26" priority="3">
       <formula>G1="X"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="4">
+    <cfRule type="expression" dxfId="25" priority="4">
       <formula>G1="Y"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="5">
+    <cfRule type="expression" dxfId="24" priority="5">
       <formula>G1="Z"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="6">
+    <cfRule type="expression" dxfId="23" priority="6">
       <formula>G1="B"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H80:H95">
-    <cfRule type="expression" dxfId="6" priority="2">
+    <cfRule type="expression" dxfId="22" priority="2">
       <formula>$H$51&lt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C13">
-    <cfRule type="expression" dxfId="5" priority="276">
+    <cfRule type="expression" dxfId="21" priority="276">
       <formula>OR($C$13&gt;=$C$9, $C$13&gt;=$C$40)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14">
-    <cfRule type="expression" dxfId="4" priority="277">
+    <cfRule type="expression" dxfId="20" priority="277">
       <formula>OR($C$14&gt;=$C$10, $C$14&gt;=$C$40)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C17">
-    <cfRule type="expression" dxfId="3" priority="278">
+    <cfRule type="expression" dxfId="19" priority="278">
       <formula>OR($C$17&lt;=0, $C$17&gt;=($C$9-#REF!)/2, $C$17&gt;=($C$36-#REF!)/2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H77">
-    <cfRule type="expression" dxfId="2" priority="279">
+    <cfRule type="expression" dxfId="18" priority="279">
       <formula>$H$77&lt;=$C$27/2+$C$28</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C27">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="17" priority="1">
       <formula>OR($C$27&lt;=0, $C$27&gt;$C$26)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -22474,12 +22485,12 @@
   </sheetData>
   <phoneticPr fontId="1"/>
   <conditionalFormatting sqref="B2:D42">
-    <cfRule type="expression" dxfId="39" priority="2">
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>$A2&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:N42">
-    <cfRule type="expression" dxfId="38" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>$A2&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
fix calculation for dimple
</commit_message>
<xml_diff>
--- a/Mould_Database/Mould_DB.xlsx
+++ b/Mould_Database/Mould_DB.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user01\Documents\GitHub\mould\Mould_Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFF50E9B-C09B-47BF-A759-B87F0D86EB12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67E88BC5-D04E-414A-B5A7-1CB8B007E14D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9360" yWindow="0" windowWidth="19440" windowHeight="15600" tabRatio="638" firstSheet="13" activeTab="15" xr2:uid="{331D296A-DE97-4357-9338-22F5C8F49D08}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" tabRatio="638" firstSheet="13" activeTab="15" xr2:uid="{331D296A-DE97-4357-9338-22F5C8F49D08}"/>
   </bookViews>
   <sheets>
     <sheet name="master" sheetId="2" r:id="rId1"/>
@@ -72,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="479">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="490">
   <si>
     <t>列1</t>
   </si>
@@ -12227,6 +12227,170 @@
     </rPh>
     <rPh sb="8" eb="10">
       <t>チョッケイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>G57X</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>G57Y</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <t>g</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="メイリオ"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>tx</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <t>g</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="メイリオ"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>tz</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <t>g'</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="メイリオ"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>tx</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <t>g'</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="メイリオ"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>tz</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <t>傾け前後g</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="メイリオ"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>tx</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="メイリオ"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>移動距離</t>
+    </r>
+    <rPh sb="0" eb="1">
+      <t>カタム</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>ゼンゴ</t>
+    </rPh>
+    <rPh sb="7" eb="11">
+      <t>イドウキョ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>G57X（傾け前）fromテーブル中心</t>
+    <rPh sb="5" eb="6">
+      <t>カタム</t>
+    </rPh>
+    <rPh sb="7" eb="8">
+      <t>マエ</t>
+    </rPh>
+    <rPh sb="17" eb="19">
+      <t>チュウシン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>G57Z（傾け前）fromテーブル中心</t>
+    <rPh sb="5" eb="6">
+      <t>カタム</t>
+    </rPh>
+    <rPh sb="7" eb="8">
+      <t>マエ</t>
+    </rPh>
+    <rPh sb="17" eb="19">
+      <t>チュウシン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>G57X（傾け後）fromテーブル中心</t>
+    <rPh sb="5" eb="6">
+      <t>カタム</t>
+    </rPh>
+    <rPh sb="7" eb="8">
+      <t>ゴ</t>
+    </rPh>
+    <rPh sb="17" eb="19">
+      <t>チュウシン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>G57Z（傾け後）fromテーブル中心</t>
+    <rPh sb="5" eb="6">
+      <t>カタム</t>
+    </rPh>
+    <rPh sb="7" eb="8">
+      <t>ゴ</t>
+    </rPh>
+    <rPh sb="17" eb="19">
+      <t>チュウシン</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -13046,111 +13210,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
@@ -13358,6 +13417,111 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
         </patternFill>
       </fill>
     </dxf>
@@ -15834,71 +15998,71 @@
   </sheetData>
   <phoneticPr fontId="1"/>
   <conditionalFormatting sqref="C3">
-    <cfRule type="expression" dxfId="16" priority="6">
+    <cfRule type="expression" dxfId="54" priority="6">
       <formula>G9^2&lt;4*G10^2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4">
-    <cfRule type="expression" dxfId="15" priority="5">
+    <cfRule type="expression" dxfId="53" priority="5">
       <formula>$C$4&lt;=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C5">
-    <cfRule type="expression" dxfId="14" priority="1">
+    <cfRule type="expression" dxfId="52" priority="1">
       <formula>C5&lt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6">
-    <cfRule type="expression" dxfId="13" priority="10">
+    <cfRule type="expression" dxfId="51" priority="10">
       <formula>OR(C5&gt;C6, C6&lt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7">
-    <cfRule type="expression" dxfId="12" priority="9">
+    <cfRule type="expression" dxfId="50" priority="9">
       <formula>AND(C7&lt;&gt;330, C7&lt;&gt;270, C7&lt;&gt;250)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="expression" dxfId="11" priority="8">
+    <cfRule type="expression" dxfId="49" priority="8">
       <formula>C8&lt;&gt;40</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9">
-    <cfRule type="expression" dxfId="10" priority="7">
+    <cfRule type="expression" dxfId="48" priority="7">
       <formula>C9&lt;&gt;100</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K3:K4">
-    <cfRule type="expression" dxfId="9" priority="15">
+    <cfRule type="expression" dxfId="47" priority="15">
       <formula>OR(($K$8&gt;($C$5+$C$6-2*$C$7)),$K$3&lt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M3:M32">
-    <cfRule type="expression" dxfId="8" priority="2">
+    <cfRule type="expression" dxfId="46" priority="2">
       <formula>Q3&gt;=1000000</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="13">
+    <cfRule type="expression" dxfId="45" priority="13">
       <formula>Q3=MIN($Q$3:$Q32)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O3:O32">
-    <cfRule type="expression" dxfId="6" priority="3">
+    <cfRule type="expression" dxfId="44" priority="3">
       <formula>Q3&gt;=1000000</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="12">
+    <cfRule type="expression" dxfId="43" priority="12">
       <formula>Q3=MIN($Q$3:$Q32)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P3:P32">
-    <cfRule type="expression" dxfId="4" priority="4">
+    <cfRule type="expression" dxfId="42" priority="4">
       <formula>Q3&gt;=1000000</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="11">
+    <cfRule type="expression" dxfId="41" priority="11">
       <formula>Q3=MIN($Q$3:$Q32)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R3:R32">
-    <cfRule type="expression" dxfId="2" priority="14">
+    <cfRule type="expression" dxfId="40" priority="14">
       <formula>Q3=MIN($Q$3:$Q32)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -15914,8 +16078,8 @@
   <sheetPr codeName="Sheet16"/>
   <dimension ref="A1:R170"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="I80" sqref="I80"/>
+    <sheetView tabSelected="1" topLeftCell="D70" workbookViewId="0">
+      <selection activeCell="F89" sqref="F89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.4"/>
@@ -18431,6 +18595,12 @@
       </c>
     </row>
     <row r="69" spans="2:14" x14ac:dyDescent="0.4">
+      <c r="B69" s="53" t="s">
+        <v>479</v>
+      </c>
+      <c r="C69" s="57">
+        <v>-561.11400000000003</v>
+      </c>
       <c r="E69" s="55" t="s">
         <v>428</v>
       </c>
@@ -18464,6 +18634,12 @@
       </c>
     </row>
     <row r="70" spans="2:14" x14ac:dyDescent="0.4">
+      <c r="B70" s="53" t="s">
+        <v>480</v>
+      </c>
+      <c r="C70" s="57">
+        <v>-648.33199999999999</v>
+      </c>
       <c r="E70" s="55" t="s">
         <v>385</v>
       </c>
@@ -19206,7 +19382,24 @@
         <v>8995.6564181061131</v>
       </c>
     </row>
-    <row r="97" spans="11:14" x14ac:dyDescent="0.4">
+    <row r="97" spans="5:14" x14ac:dyDescent="0.4">
+      <c r="E97" s="55" t="s">
+        <v>481</v>
+      </c>
+      <c r="F97" s="61" t="s">
+        <v>486</v>
+      </c>
+      <c r="G97" s="65" t="s">
+        <v>206</v>
+      </c>
+      <c r="H97" s="82">
+        <f>$C$69-$C64</f>
+        <v>-11.095000000000027</v>
+      </c>
+      <c r="I97" s="82">
+        <f>$C$64+H97</f>
+        <v>-561.11400000000003</v>
+      </c>
       <c r="K97" s="55">
         <f t="shared" si="3"/>
         <v>97</v>
@@ -19222,7 +19415,24 @@
         <v>8992.3094054643298</v>
       </c>
     </row>
-    <row r="98" spans="11:14" x14ac:dyDescent="0.4">
+    <row r="98" spans="5:14" x14ac:dyDescent="0.4">
+      <c r="E98" s="55" t="s">
+        <v>482</v>
+      </c>
+      <c r="F98" s="61" t="s">
+        <v>487</v>
+      </c>
+      <c r="G98" s="65" t="s">
+        <v>203</v>
+      </c>
+      <c r="H98" s="82">
+        <f>$H$3</f>
+        <v>500.01603829462465</v>
+      </c>
+      <c r="I98" s="82">
+        <f>$C$65+H98</f>
+        <v>-649.95796170537528</v>
+      </c>
       <c r="K98" s="55">
         <f t="shared" si="3"/>
         <v>98</v>
@@ -19238,7 +19448,24 @@
         <v>3.7189029353147718E-2</v>
       </c>
     </row>
-    <row r="99" spans="11:14" x14ac:dyDescent="0.4">
+    <row r="99" spans="5:14" x14ac:dyDescent="0.4">
+      <c r="E99" s="55" t="s">
+        <v>483</v>
+      </c>
+      <c r="F99" s="61" t="s">
+        <v>488</v>
+      </c>
+      <c r="G99" s="65" t="s">
+        <v>206</v>
+      </c>
+      <c r="H99" s="82">
+        <f ca="1">$H$97*$N$101+$H$98*$N$100</f>
+        <v>7.4967373522236862</v>
+      </c>
+      <c r="I99" s="82">
+        <f ca="1">$C$64+H99</f>
+        <v>-542.5222626477763</v>
+      </c>
       <c r="K99" s="55">
         <f t="shared" si="3"/>
         <v>99</v>
@@ -19254,7 +19481,24 @@
         <v>3.7171899126953054E-2</v>
       </c>
     </row>
-    <row r="100" spans="11:14" x14ac:dyDescent="0.4">
+    <row r="100" spans="5:14" x14ac:dyDescent="0.4">
+      <c r="E100" s="55" t="s">
+        <v>484</v>
+      </c>
+      <c r="F100" s="61" t="s">
+        <v>489</v>
+      </c>
+      <c r="G100" s="65" t="s">
+        <v>203</v>
+      </c>
+      <c r="H100" s="82">
+        <f ca="1">-$H$97*$N$100+$H$98*$N$101</f>
+        <v>500.08292962860008</v>
+      </c>
+      <c r="I100" s="82">
+        <f ca="1">$C$65+H100</f>
+        <v>-649.89107037139979</v>
+      </c>
       <c r="K100" s="55">
         <f t="shared" si="3"/>
         <v>100</v>
@@ -19270,7 +19514,17 @@
         <v>3.7166950783010577E-2</v>
       </c>
     </row>
-    <row r="101" spans="11:14" x14ac:dyDescent="0.4">
+    <row r="101" spans="5:14" x14ac:dyDescent="0.4">
+      <c r="F101" s="61" t="s">
+        <v>485</v>
+      </c>
+      <c r="G101" s="65" t="s">
+        <v>206</v>
+      </c>
+      <c r="H101" s="82">
+        <f ca="1">$H$99-$H$97</f>
+        <v>18.591737352223713</v>
+      </c>
       <c r="K101" s="55">
         <f t="shared" si="3"/>
         <v>101</v>
@@ -19286,7 +19540,17 @@
         <v>0.9993090701927474</v>
       </c>
     </row>
-    <row r="102" spans="11:14" x14ac:dyDescent="0.4">
+    <row r="102" spans="5:14" x14ac:dyDescent="0.4">
+      <c r="F102" s="61" t="s">
+        <v>485</v>
+      </c>
+      <c r="G102" s="65" t="s">
+        <v>203</v>
+      </c>
+      <c r="H102" s="82">
+        <f ca="1">$H$100-$H$98</f>
+        <v>6.6891333975434009E-2</v>
+      </c>
       <c r="K102" s="55">
         <f t="shared" si="3"/>
         <v>102</v>
@@ -19302,7 +19566,7 @@
         <v>8844.4037000000008</v>
       </c>
     </row>
-    <row r="103" spans="11:14" x14ac:dyDescent="0.4">
+    <row r="103" spans="5:14" x14ac:dyDescent="0.4">
       <c r="K103" s="55">
         <f t="shared" si="3"/>
         <v>103</v>
@@ -19318,7 +19582,7 @@
         <v>8844.6194000000014</v>
       </c>
     </row>
-    <row r="104" spans="11:14" x14ac:dyDescent="0.4">
+    <row r="104" spans="5:14" x14ac:dyDescent="0.4">
       <c r="K104" s="55">
         <f t="shared" si="2"/>
         <v>104</v>
@@ -19334,7 +19598,7 @@
         <v>8842.1260074066122</v>
       </c>
     </row>
-    <row r="105" spans="11:14" x14ac:dyDescent="0.4">
+    <row r="105" spans="5:14" x14ac:dyDescent="0.4">
       <c r="K105" s="55">
         <f t="shared" si="2"/>
         <v>105</v>
@@ -19350,7 +19614,7 @@
         <v>8838.9692164060452</v>
       </c>
     </row>
-    <row r="106" spans="11:14" x14ac:dyDescent="0.4">
+    <row r="106" spans="5:14" x14ac:dyDescent="0.4">
       <c r="K106" s="55">
         <f t="shared" si="2"/>
         <v>106</v>
@@ -19363,7 +19627,7 @@
         <v>3.1567910005669546E-2</v>
       </c>
     </row>
-    <row r="107" spans="11:14" x14ac:dyDescent="0.4">
+    <row r="107" spans="5:14" x14ac:dyDescent="0.4">
       <c r="K107" s="55">
         <f t="shared" si="2"/>
         <v>107</v>
@@ -19379,7 +19643,7 @@
         <v>3.1557430117010586E-2</v>
       </c>
     </row>
-    <row r="108" spans="11:14" x14ac:dyDescent="0.4">
+    <row r="108" spans="5:14" x14ac:dyDescent="0.4">
       <c r="K108" s="55">
         <f>ROW(K108)</f>
         <v>108</v>
@@ -19395,7 +19659,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="109" spans="11:14" x14ac:dyDescent="0.4">
+    <row r="109" spans="5:14" x14ac:dyDescent="0.4">
       <c r="K109" s="55">
         <f t="shared" si="2"/>
         <v>109</v>
@@ -19411,7 +19675,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="110" spans="11:14" x14ac:dyDescent="0.4">
+    <row r="110" spans="5:14" x14ac:dyDescent="0.4">
       <c r="K110" s="55">
         <f t="shared" si="2"/>
         <v>110</v>
@@ -19427,7 +19691,7 @@
         <v>21.495936780292737</v>
       </c>
     </row>
-    <row r="111" spans="11:14" x14ac:dyDescent="0.4">
+    <row r="111" spans="5:14" x14ac:dyDescent="0.4">
       <c r="K111" s="55">
         <f t="shared" si="2"/>
         <v>111</v>
@@ -19443,7 +19707,7 @@
         <v>29.502662230977563</v>
       </c>
     </row>
-    <row r="112" spans="11:14" x14ac:dyDescent="0.4">
+    <row r="112" spans="5:14" x14ac:dyDescent="0.4">
       <c r="K112" s="55">
         <f t="shared" si="2"/>
         <v>112</v>
@@ -20130,191 +20394,191 @@
   </sheetData>
   <phoneticPr fontId="1"/>
   <conditionalFormatting sqref="C3">
-    <cfRule type="expression" dxfId="54" priority="123">
+    <cfRule type="expression" dxfId="39" priority="123">
       <formula>$C$3&gt;2*N151</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4">
-    <cfRule type="expression" dxfId="53" priority="43">
+    <cfRule type="expression" dxfId="38" priority="43">
       <formula>C4&lt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6">
-    <cfRule type="expression" dxfId="52" priority="19">
+    <cfRule type="expression" dxfId="37" priority="19">
       <formula>$C$6&lt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9">
-    <cfRule type="expression" dxfId="51" priority="47">
+    <cfRule type="expression" dxfId="36" priority="47">
       <formula>$C$9&lt;=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10:C11">
-    <cfRule type="expression" dxfId="50" priority="20">
+    <cfRule type="expression" dxfId="35" priority="20">
       <formula>$C$10&lt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15">
-    <cfRule type="expression" dxfId="49" priority="98">
+    <cfRule type="expression" dxfId="34" priority="98">
       <formula>OR(C15&lt;=0, C15&gt;Q2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="expression" dxfId="48" priority="42">
+    <cfRule type="expression" dxfId="33" priority="42">
       <formula>C35&lt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="expression" dxfId="47" priority="57">
+    <cfRule type="expression" dxfId="32" priority="57">
       <formula>OR($C$36&lt;0, $C$36&gt;=$C$9)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="expression" dxfId="46" priority="16">
+    <cfRule type="expression" dxfId="31" priority="16">
       <formula>OR($C$37&lt;0, $C$37&gt;=$C$10)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38">
-    <cfRule type="expression" dxfId="45" priority="120">
+    <cfRule type="expression" dxfId="30" priority="120">
       <formula>OR(C38&lt;0, C38&gt;=C9)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C39">
-    <cfRule type="expression" dxfId="44" priority="127">
+    <cfRule type="expression" dxfId="29" priority="127">
       <formula>OR(C39&lt;0, C39&gt;=C4)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C42">
-    <cfRule type="expression" dxfId="43" priority="128">
+    <cfRule type="expression" dxfId="28" priority="128">
       <formula>OR(C42&lt;0, C42&gt;=C4)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C59">
-    <cfRule type="expression" dxfId="42" priority="51">
+    <cfRule type="expression" dxfId="27" priority="51">
       <formula>AND(C59&lt;&gt;330, C59&lt;&gt;270, C59&lt;&gt;250)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C60">
-    <cfRule type="expression" dxfId="41" priority="50">
+    <cfRule type="expression" dxfId="26" priority="50">
       <formula>C60&lt;&gt;40</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C63">
-    <cfRule type="expression" dxfId="40" priority="27">
+    <cfRule type="expression" dxfId="25" priority="27">
       <formula>OR(C63&gt;0, ABS(ABS(C63)-740)&gt;=1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C64">
-    <cfRule type="expression" dxfId="39" priority="40">
+    <cfRule type="expression" dxfId="24" priority="40">
       <formula>OR(C64&gt;0, ABS(ABS(C64)-550)&gt;=1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C65">
-    <cfRule type="expression" dxfId="38" priority="33">
+    <cfRule type="expression" dxfId="23" priority="33">
       <formula>OR(C65&gt;0, ABS(ABS(C65)-1150)&gt;=1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C66">
-    <cfRule type="expression" dxfId="37" priority="39">
+    <cfRule type="expression" dxfId="22" priority="39">
       <formula>OR(ABS(C66)&gt;=0.2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H48">
-    <cfRule type="expression" dxfId="36" priority="23">
+    <cfRule type="expression" dxfId="21" priority="23">
       <formula>OR($H$48&lt;=1, INT($H$48)&lt;&gt;$H$48)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H52">
-    <cfRule type="expression" dxfId="35" priority="15">
+    <cfRule type="expression" dxfId="20" priority="15">
       <formula>ISERROR(INDIRECT($H$52&amp;"!$G$45"))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C25">
-    <cfRule type="expression" dxfId="34" priority="236">
+    <cfRule type="expression" dxfId="19" priority="236">
       <formula>OR(C25-QUOTIENT(C25,1)&lt;&gt;0, C25&lt;0, C25&gt;$C$67)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H50">
-    <cfRule type="expression" dxfId="33" priority="11">
+    <cfRule type="expression" dxfId="18" priority="11">
       <formula>$H$50&lt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H78 H51:H52 H54:H72">
-    <cfRule type="expression" dxfId="32" priority="10">
+    <cfRule type="expression" dxfId="17" priority="10">
       <formula>$H$51&lt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C23">
-    <cfRule type="expression" dxfId="31" priority="254">
+    <cfRule type="expression" dxfId="16" priority="254">
       <formula>OR($C$23&lt;=0, MOD($C$23,$C$22)&lt;&gt;0, $C$23&gt;=#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C26">
-    <cfRule type="expression" dxfId="30" priority="262">
+    <cfRule type="expression" dxfId="15" priority="262">
       <formula>OR($C$26&lt;=0, $C$26&gt;=MIN($C$23, $C$24))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N128:N133">
-    <cfRule type="expression" dxfId="29" priority="9">
+    <cfRule type="expression" dxfId="14" priority="9">
       <formula>$H$51&lt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N134:N141">
-    <cfRule type="expression" dxfId="28" priority="8">
+    <cfRule type="expression" dxfId="13" priority="8">
       <formula>$H$51&lt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C16">
-    <cfRule type="expression" dxfId="27" priority="274">
+    <cfRule type="expression" dxfId="12" priority="274">
       <formula>OR(C16&lt;=0, C16+C15&gt;Q2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G1048576">
-    <cfRule type="expression" dxfId="26" priority="3">
+    <cfRule type="expression" dxfId="11" priority="3">
       <formula>G1="X"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="4">
+    <cfRule type="expression" dxfId="10" priority="4">
       <formula>G1="Y"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="5">
+    <cfRule type="expression" dxfId="9" priority="5">
       <formula>G1="Z"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="23" priority="6">
+    <cfRule type="expression" dxfId="8" priority="6">
       <formula>G1="B"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H80:H95">
-    <cfRule type="expression" dxfId="22" priority="2">
+    <cfRule type="expression" dxfId="7" priority="2">
       <formula>$H$51&lt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C13">
-    <cfRule type="expression" dxfId="21" priority="276">
+    <cfRule type="expression" dxfId="6" priority="276">
       <formula>OR($C$13&gt;=$C$9, $C$13&gt;=$C$40)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14">
-    <cfRule type="expression" dxfId="20" priority="277">
+    <cfRule type="expression" dxfId="5" priority="277">
       <formula>OR($C$14&gt;=$C$10, $C$14&gt;=$C$40)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C17">
-    <cfRule type="expression" dxfId="19" priority="278">
+    <cfRule type="expression" dxfId="4" priority="278">
       <formula>OR($C$17&lt;=0, $C$17&gt;=($C$9-#REF!)/2, $C$17&gt;=($C$36-#REF!)/2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H77">
-    <cfRule type="expression" dxfId="18" priority="279">
+    <cfRule type="expression" dxfId="3" priority="279">
       <formula>$H$77&lt;=$C$27/2+$C$28</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C27">
-    <cfRule type="expression" dxfId="17" priority="1">
+    <cfRule type="expression" dxfId="2" priority="1">
       <formula>OR($C$27&lt;=0, $C$27&gt;$C$26)</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation imeMode="disabled" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C58:C67 H78 N128:N141 C47:C50 C53:C56 H54:H72 H80:H95 G1:G1048576 C3:C32" xr:uid="{5A8FA8E9-E7FC-48D2-B40E-E90D3C7D1F03}"/>
+    <dataValidation imeMode="disabled" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C58:C67 H78 N128:N141 C47:C50 C53:C56 H54:H72 H80:H95 C3:C32 G1:G1048576" xr:uid="{5A8FA8E9-E7FC-48D2-B40E-E90D3C7D1F03}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>